<commit_message>
Default values for excel
</commit_message>
<xml_diff>
--- a/SEBAL/InputEXCEL_v3_3_7.xlsx
+++ b/SEBAL/InputEXCEL_v3_3_7.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5748" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5748" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General_Input" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="91">
   <si>
     <t>InputMap</t>
   </si>
@@ -951,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1013,36 +1013,36 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="2" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>82</v>
+      <c r="B2" s="4">
+        <v>25.8</v>
+      </c>
+      <c r="C2" s="4">
+        <v>20.93</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44</v>
+      </c>
+      <c r="E2" s="4">
+        <v>70.22</v>
       </c>
       <c r="F2" s="4">
         <v>2</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>84</v>
+      <c r="G2" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.38</v>
       </c>
       <c r="I2" s="4">
         <v>1</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>85</v>
+      <c r="J2" s="4">
+        <v>310</v>
       </c>
       <c r="K2" s="4">
         <v>0.7</v>
@@ -1050,8 +1050,8 @@
       <c r="L2" s="4">
         <v>1</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>86</v>
+      <c r="M2" s="4">
+        <v>569</v>
       </c>
       <c r="N2" s="4">
         <v>0.75</v>
@@ -1231,7 +1231,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1275,15 +1275,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>88</v>
+      <c r="B2" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.4</v>
       </c>
       <c r="D2" s="4">
         <v>0.02</v>
@@ -1291,11 +1291,11 @@
       <c r="E2" s="4">
         <v>0.02</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>90</v>
+      <c r="F2" s="4">
+        <v>0.32</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.04</v>
       </c>
       <c r="H2" s="4">
         <v>0.5</v>
@@ -1303,12 +1303,6 @@
       <c r="I2" s="4">
         <v>2.5</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
@@ -1850,7 +1844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>